<commit_message>
More Paramter Tuning - Some Succesful Algorithms found
</commit_message>
<xml_diff>
--- a/Comp Int Report/Data.xlsx
+++ b/Comp Int Report/Data.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11670" windowHeight="4455" firstSheet="3" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11670" windowHeight="4455" firstSheet="3" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="All Permutations,initial weight" sheetId="1" r:id="rId1"/>
     <sheet name="Best Permutation" sheetId="2" r:id="rId2"/>
     <sheet name="Mutation Rate + Change" sheetId="3" r:id="rId3"/>
     <sheet name="Hidden Layers" sheetId="4" r:id="rId4"/>
+    <sheet name="U-R-B" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="55">
   <si>
     <t>SP, R, Bound A</t>
   </si>
@@ -174,6 +175,24 @@
   </si>
   <si>
     <t>MR 0.2, MC 0.5</t>
+  </si>
+  <si>
+    <t>Bound -1, 1</t>
+  </si>
+  <si>
+    <t>6 L, 40 P, MR 0.085, MC 1.03, 1.5 B, U, T, MM, TS 20</t>
+  </si>
+  <si>
+    <t>10 L, 40 P, MR 0.085, MC 1.03, 1.5 B, U, T, MM, TS 20</t>
+  </si>
+  <si>
+    <t>6 L, 80 P, MR 0.085, MC 1.03, 1.5 B, U, T, MM, TS 40</t>
+  </si>
+  <si>
+    <t>6 L, 80 P, MR 0.1, MC 1.03, 1.5 B, U, T, MM, TS 40</t>
+  </si>
+  <si>
+    <t>6 L, 80 P, MR 0.085, MC 1.03, 1 B, U, T, MM, TS 40</t>
   </si>
 </sst>
 </file>
@@ -556,7 +575,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:S25"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="A4" sqref="A4:A25"/>
     </sheetView>
   </sheetViews>
@@ -1852,8 +1871,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I26"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B26"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1862,6 +1881,7 @@
     <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -1880,7 +1900,9 @@
       <c r="F2" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="G2" s="3"/>
+      <c r="G2" s="3" t="s">
+        <v>49</v>
+      </c>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
     </row>
@@ -1903,6 +1925,9 @@
       <c r="F3">
         <v>0.136475193582974</v>
       </c>
+      <c r="G3">
+        <v>0.12786197771667401</v>
+      </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -2093,7 +2118,7 @@
         <v>9.4635209148676971E-2</v>
       </c>
       <c r="C13" s="1">
-        <f t="shared" ref="C13:I13" si="0">SUM(C3:C12)/10</f>
+        <f t="shared" ref="C13:F13" si="0">SUM(C3:C12)/10</f>
         <v>0.1000117221234658</v>
       </c>
       <c r="D13" s="1">
@@ -2121,7 +2146,7 @@
         <v>0</v>
       </c>
       <c r="C14" s="4">
-        <f t="shared" ref="C14:I14" si="1">(($B$13-C13)/$B$13)</f>
+        <f t="shared" ref="C14:F14" si="1">(($B$13-C13)/$B$13)</f>
         <v>-5.6813029982763011E-2</v>
       </c>
       <c r="D14" s="4">
@@ -2357,7 +2382,7 @@
         <v>0.21711500449303817</v>
       </c>
       <c r="E25" s="1">
-        <f t="shared" ref="E25:I25" si="4">SUM(E15:E23)/10</f>
+        <f t="shared" ref="E25:F25" si="4">SUM(E15:E23)/10</f>
         <v>0.2236941764508133</v>
       </c>
       <c r="F25" s="1">
@@ -2377,7 +2402,7 @@
         <v>0</v>
       </c>
       <c r="C26" s="4">
-        <f t="shared" ref="C26:I26" si="5">(($B$25-C25)/$B$25)</f>
+        <f t="shared" ref="C26:F26" si="5">(($B$25-C25)/$B$25)</f>
         <v>-3.9565045655742754E-3</v>
       </c>
       <c r="D26" s="4">
@@ -2649,7 +2674,7 @@
         <v>9.4635209148676971E-2</v>
       </c>
       <c r="C13" s="1">
-        <f t="shared" ref="C13:H13" si="0">SUM(C3:C12)/10</f>
+        <f t="shared" ref="C13:F13" si="0">SUM(C3:C12)/10</f>
         <v>0.11053547885824562</v>
       </c>
       <c r="D13" s="1">
@@ -2694,7 +2719,7 @@
         <v>0</v>
       </c>
       <c r="C14" s="4">
-        <f t="shared" ref="C14:H14" si="6">(($B$13-C13)/$B$13)</f>
+        <f t="shared" ref="C14:F14" si="6">(($B$13-C13)/$B$13)</f>
         <v>-0.16801642700010813</v>
       </c>
       <c r="D14" s="4">
@@ -3005,7 +3030,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D5" workbookViewId="0">
+    <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
@@ -3682,4 +3707,510 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:H24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="F3" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="45" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="46" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="45" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="43" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3">
+        <v>1.8448958522437098E-2</v>
+      </c>
+      <c r="C3">
+        <v>2.5400598984586201E-2</v>
+      </c>
+      <c r="D3">
+        <v>8.8830658985836905E-2</v>
+      </c>
+      <c r="E3">
+        <v>7.1162641998232204E-2</v>
+      </c>
+      <c r="F3">
+        <v>4.88181077743318E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4">
+        <v>5.3146994221677797E-2</v>
+      </c>
+      <c r="C4">
+        <v>4.5530257478257702E-2</v>
+      </c>
+      <c r="D4">
+        <v>9.3202815634529396E-2</v>
+      </c>
+      <c r="E4">
+        <v>6.7293876570999001E-2</v>
+      </c>
+      <c r="F4">
+        <v>9.7948943059156204E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5">
+        <v>6.0715057011706097E-2</v>
+      </c>
+      <c r="C5">
+        <v>7.8116730402077394E-2</v>
+      </c>
+      <c r="D5">
+        <v>2.6439824718711601E-2</v>
+      </c>
+      <c r="E5">
+        <v>1.3195647226609699E-2</v>
+      </c>
+      <c r="F5">
+        <v>7.8010256157927907E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6">
+        <v>0.118160526385896</v>
+      </c>
+      <c r="C6">
+        <v>4.5551617871417698E-2</v>
+      </c>
+      <c r="D6">
+        <v>5.1774667805565201E-2</v>
+      </c>
+      <c r="E6">
+        <v>6.4113256819364098E-2</v>
+      </c>
+      <c r="F6">
+        <v>3.9556998534261298E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7">
+        <v>4.1070438641174302E-2</v>
+      </c>
+      <c r="C7">
+        <v>7.0906905145906807E-2</v>
+      </c>
+      <c r="D7">
+        <v>3.4077479089814601E-2</v>
+      </c>
+      <c r="E7">
+        <v>2.2283582507905901E-2</v>
+      </c>
+      <c r="F7">
+        <v>5.8687660147565102E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8">
+        <v>3.9183229092567801E-2</v>
+      </c>
+      <c r="C8">
+        <v>2.6452143732452998E-2</v>
+      </c>
+      <c r="D8">
+        <v>5.4484502854665898E-2</v>
+      </c>
+      <c r="E8">
+        <v>0.127001872926154</v>
+      </c>
+      <c r="F8">
+        <v>6.2726113901063807E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9">
+        <v>0.110373119612226</v>
+      </c>
+      <c r="C9">
+        <v>0.10228949529452</v>
+      </c>
+      <c r="D9">
+        <v>4.6096008407671897E-2</v>
+      </c>
+      <c r="E9">
+        <v>6.0283148352783297E-2</v>
+      </c>
+      <c r="F9">
+        <v>2.3873623288709199E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10">
+        <v>9.7138351644410301E-2</v>
+      </c>
+      <c r="C10">
+        <v>0.10494767284445899</v>
+      </c>
+      <c r="D10">
+        <v>5.03467862673194E-2</v>
+      </c>
+      <c r="E10">
+        <v>5.02629547801028E-2</v>
+      </c>
+      <c r="F10">
+        <v>6.8511794755148903E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11">
+        <v>8.87613955906532E-2</v>
+      </c>
+      <c r="C11">
+        <v>0.100056116758379</v>
+      </c>
+      <c r="D11">
+        <v>6.8692840252109102E-2</v>
+      </c>
+      <c r="E11">
+        <v>5.19806736783174E-2</v>
+      </c>
+      <c r="F11">
+        <v>6.4836587478437097E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12">
+        <v>2.15752520110159E-2</v>
+      </c>
+      <c r="C12">
+        <v>5.3521347212742897E-2</v>
+      </c>
+      <c r="D12">
+        <v>1.6206259104558699E-2</v>
+      </c>
+      <c r="E12">
+        <v>9.2894448553123801E-2</v>
+      </c>
+      <c r="F12">
+        <v>5.5433159947090797E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="1">
+        <f>SUM(B3:B12)/10</f>
+        <v>6.485733227337645E-2</v>
+      </c>
+      <c r="C13" s="1">
+        <f t="shared" ref="C13:H13" si="0">SUM(C3:C12)/10</f>
+        <v>6.5277288572479983E-2</v>
+      </c>
+      <c r="D13" s="1">
+        <f t="shared" si="0"/>
+        <v>5.301518431207828E-2</v>
+      </c>
+      <c r="E13" s="1">
+        <f t="shared" si="0"/>
+        <v>6.2047210341359217E-2</v>
+      </c>
+      <c r="F13" s="1">
+        <f t="shared" si="0"/>
+        <v>5.9840324504369199E-2</v>
+      </c>
+      <c r="G13" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H13" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14">
+        <v>3.7120195375204897E-2</v>
+      </c>
+      <c r="C14">
+        <v>0.13486102425906099</v>
+      </c>
+      <c r="D14">
+        <v>0.24082342847048499</v>
+      </c>
+      <c r="E14">
+        <v>0.13063843128783001</v>
+      </c>
+      <c r="F14">
+        <v>8.7569988677640806E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15">
+        <v>0.13302564564081401</v>
+      </c>
+      <c r="C15">
+        <v>9.3404340801820696E-2</v>
+      </c>
+      <c r="D15">
+        <v>0.22964205217158401</v>
+      </c>
+      <c r="E15">
+        <v>0.122911054802745</v>
+      </c>
+      <c r="F15">
+        <v>0.20124991905364101</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16">
+        <v>9.2321599596660905E-2</v>
+      </c>
+      <c r="C16">
+        <v>9.5711428605484497E-2</v>
+      </c>
+      <c r="D16">
+        <v>0.10864921581539801</v>
+      </c>
+      <c r="E16">
+        <v>2.0286304579862399E-2</v>
+      </c>
+      <c r="F16">
+        <v>0.158044471354466</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17">
+        <v>0.26578282124488201</v>
+      </c>
+      <c r="C17">
+        <v>5.17897770888084E-2</v>
+      </c>
+      <c r="D17">
+        <v>0.13671846736194401</v>
+      </c>
+      <c r="E17">
+        <v>0.23374023638882599</v>
+      </c>
+      <c r="F17">
+        <v>6.6516874783178706E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18">
+        <v>6.8045597190145898E-2</v>
+      </c>
+      <c r="C18">
+        <v>0.183744124619525</v>
+      </c>
+      <c r="D18">
+        <v>8.4868648144526104E-2</v>
+      </c>
+      <c r="E18">
+        <v>0.18931857217286799</v>
+      </c>
+      <c r="F18">
+        <v>0.20337883120081801</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19">
+        <v>0.115016561403445</v>
+      </c>
+      <c r="C19">
+        <v>0.143629020005695</v>
+      </c>
+      <c r="D19">
+        <v>0.243381179453458</v>
+      </c>
+      <c r="E19">
+        <v>0.29389805342398401</v>
+      </c>
+      <c r="F19">
+        <v>0.190294276118984</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20">
+        <v>0.258440505413573</v>
+      </c>
+      <c r="C20">
+        <v>0.28964607803838299</v>
+      </c>
+      <c r="D20">
+        <v>0.13048944680434699</v>
+      </c>
+      <c r="E20">
+        <v>0.18588822637695199</v>
+      </c>
+      <c r="F20">
+        <v>5.2068521068177498E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21">
+        <v>0.18683399182624699</v>
+      </c>
+      <c r="C21">
+        <v>0.21304089521844999</v>
+      </c>
+      <c r="D21">
+        <v>0.142329557003982</v>
+      </c>
+      <c r="E21">
+        <v>0.16775580424098599</v>
+      </c>
+      <c r="F21">
+        <v>0.15547400420750801</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22">
+        <v>0.22328579006062799</v>
+      </c>
+      <c r="C22">
+        <v>0.19547067704065399</v>
+      </c>
+      <c r="D22">
+        <v>0.14511732241734099</v>
+      </c>
+      <c r="E22">
+        <v>5.3973323605312103E-2</v>
+      </c>
+      <c r="F22">
+        <v>0.14722870926951601</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B23">
+        <v>0.125533328714759</v>
+      </c>
+      <c r="C23">
+        <v>0.118441532599976</v>
+      </c>
+      <c r="D23">
+        <v>5.9532011805678499E-2</v>
+      </c>
+      <c r="E23">
+        <v>0.23212614138378401</v>
+      </c>
+      <c r="F23">
+        <v>0.13665522794867199</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B24" s="1">
+        <f>SUM(B14:B23)/10</f>
+        <v>0.15054060364663596</v>
+      </c>
+      <c r="C24" s="1">
+        <f t="shared" ref="C24:H24" si="1">SUM(C14:C23)/10</f>
+        <v>0.15197388982778576</v>
+      </c>
+      <c r="D24" s="1">
+        <f t="shared" si="1"/>
+        <v>0.15215513294487437</v>
+      </c>
+      <c r="E24" s="1">
+        <f t="shared" si="1"/>
+        <v>0.16305361482631495</v>
+      </c>
+      <c r="F24" s="1">
+        <f t="shared" si="1"/>
+        <v>0.13984808236826018</v>
+      </c>
+      <c r="G24" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H24" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Low Averages, Report has Begun
</commit_message>
<xml_diff>
--- a/Comp Int Report/Data.xlsx
+++ b/Comp Int Report/Data.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="58">
   <si>
     <t>SP, R, Bound A</t>
   </si>
@@ -180,19 +180,28 @@
     <t>Bound -1, 1</t>
   </si>
   <si>
-    <t>6 L, 40 P, MR 0.085, MC 1.03, 1.5 B, U, T, MM, TS 20</t>
-  </si>
-  <si>
-    <t>10 L, 40 P, MR 0.085, MC 1.03, 1.5 B, U, T, MM, TS 20</t>
-  </si>
-  <si>
-    <t>6 L, 80 P, MR 0.085, MC 1.03, 1.5 B, U, T, MM, TS 40</t>
-  </si>
-  <si>
-    <t>6 L, 80 P, MR 0.1, MC 1.03, 1.5 B, U, T, MM, TS 40</t>
-  </si>
-  <si>
-    <t>6 L, 80 P, MR 0.085, MC 1.03, 1 B, U, T, MM, TS 40</t>
+    <t>5 L, 200 P, MR 0.085, MC 1.03, 1.5 B, U, T, MM, TS 20</t>
+  </si>
+  <si>
+    <t>5 L, 200 P, MR 0.085, MC 1.03, 1.5 B, U, T, MM, TS 40</t>
+  </si>
+  <si>
+    <t>5 L, 200 P, MR 0.1, MC 1.03, 1.5 B, U, T, MM, TS 40</t>
+  </si>
+  <si>
+    <t>5 L, 200 P, MR 0.085, MC 1.03, 1 B, U, T, MM, TS 40</t>
+  </si>
+  <si>
+    <t>6 L, 80 P, MR 0.1, MC 1.03, 1 B, U, T, MM, TS 40</t>
+  </si>
+  <si>
+    <t>10 L, 80 P, MR 0.1, MC 1.03, 1 B, U, T, MM, TS 40</t>
+  </si>
+  <si>
+    <t>10 L, 200 P, MR 0.15, MC 1.05, 1B, U, T, MM, TS 100</t>
+  </si>
+  <si>
+    <t>10 L, 200 P, MR 0.1, MC 1.03, 1B, U, T, MM, TS 100</t>
   </si>
 </sst>
 </file>
@@ -3711,10 +3720,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:H24"/>
+  <dimension ref="A2:L24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F3" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3724,26 +3733,40 @@
     <col min="4" max="4" width="46" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="45" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="43" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="41.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="43" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>50</v>
       </c>
       <c r="C2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" t="s">
         <v>51</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>52</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>53</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H2" t="s">
+        <v>55</v>
+      </c>
+      <c r="I2" t="s">
+        <v>57</v>
+      </c>
+      <c r="J2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>16</v>
       </c>
@@ -3762,8 +3785,17 @@
       <c r="F3">
         <v>4.88181077743318E-2</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G3">
+        <v>6.5215227535312101E-2</v>
+      </c>
+      <c r="H3">
+        <v>3.4734372136812498E-2</v>
+      </c>
+      <c r="I3">
+        <v>4.8297395184051399E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>17</v>
       </c>
@@ -3782,8 +3814,17 @@
       <c r="F4">
         <v>9.7948943059156204E-2</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G4">
+        <v>5.91455539630878E-2</v>
+      </c>
+      <c r="H4">
+        <v>4.7157949640473699E-2</v>
+      </c>
+      <c r="I4">
+        <v>2.2353670635668801E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>18</v>
       </c>
@@ -3802,8 +3843,14 @@
       <c r="F5">
         <v>7.8010256157927907E-2</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H5">
+        <v>2.0667424166192001E-2</v>
+      </c>
+      <c r="I5">
+        <v>1.9132980533019199E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>19</v>
       </c>
@@ -3822,8 +3869,14 @@
       <c r="F6">
         <v>3.9556998534261298E-2</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H6">
+        <v>3.43440433643636E-2</v>
+      </c>
+      <c r="I6">
+        <v>4.1168255637094302E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>20</v>
       </c>
@@ -3842,8 +3895,14 @@
       <c r="F7">
         <v>5.8687660147565102E-2</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H7">
+        <v>0.104021285745867</v>
+      </c>
+      <c r="I7">
+        <v>2.46391440019899E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>21</v>
       </c>
@@ -3862,8 +3921,14 @@
       <c r="F8">
         <v>6.2726113901063807E-2</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H8">
+        <v>3.9838759759506098E-2</v>
+      </c>
+      <c r="I8">
+        <v>1.15127745166188E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>22</v>
       </c>
@@ -3882,8 +3947,14 @@
       <c r="F9">
         <v>2.3873623288709199E-2</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H9">
+        <v>3.9679921844934303E-2</v>
+      </c>
+      <c r="I9">
+        <v>4.3233439442188E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>23</v>
       </c>
@@ -3902,8 +3973,14 @@
       <c r="F10">
         <v>6.8511794755148903E-2</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H10">
+        <v>1.9798855688438501E-2</v>
+      </c>
+      <c r="I10">
+        <v>4.4369412653087602E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>24</v>
       </c>
@@ -3922,8 +3999,14 @@
       <c r="F11">
         <v>6.4836587478437097E-2</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H11">
+        <v>1.9309034762565E-2</v>
+      </c>
+      <c r="I11">
+        <v>5.0305564264008298E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>25</v>
       </c>
@@ -3942,8 +4025,14 @@
       <c r="F12">
         <v>5.5433159947090797E-2</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H12">
+        <v>1.1778529248880201E-2</v>
+      </c>
+      <c r="I12">
+        <v>5.6402544378752202E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>36</v>
       </c>
@@ -3952,7 +4041,7 @@
         <v>6.485733227337645E-2</v>
       </c>
       <c r="C13" s="1">
-        <f t="shared" ref="C13:H13" si="0">SUM(C3:C12)/10</f>
+        <f t="shared" ref="C13:L13" si="0">SUM(C3:C12)/10</f>
         <v>6.5277288572479983E-2</v>
       </c>
       <c r="D13" s="1">
@@ -3969,14 +4058,30 @@
       </c>
       <c r="G13" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.2436078149839991E-2</v>
       </c>
       <c r="H13" s="1">
         <f t="shared" si="0"/>
+        <v>3.7133017635803282E-2</v>
+      </c>
+      <c r="I13" s="1">
+        <f t="shared" si="0"/>
+        <v>3.6141518124647845E-2</v>
+      </c>
+      <c r="J13" s="1">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K13" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L13" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>26</v>
       </c>
@@ -3995,8 +4100,17 @@
       <c r="F14">
         <v>8.7569988677640806E-2</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G14">
+        <v>0.16723780217697601</v>
+      </c>
+      <c r="H14">
+        <v>0.12453552917803801</v>
+      </c>
+      <c r="I14">
+        <v>8.4830002899349805E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>27</v>
       </c>
@@ -4015,8 +4129,17 @@
       <c r="F15">
         <v>0.20124991905364101</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G15">
+        <v>0.113921700913183</v>
+      </c>
+      <c r="H15">
+        <v>0.13830494182974601</v>
+      </c>
+      <c r="I15">
+        <v>6.0448279384155097E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>28</v>
       </c>
@@ -4035,8 +4158,14 @@
       <c r="F16">
         <v>0.158044471354466</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H16">
+        <v>3.9606850592967001E-2</v>
+      </c>
+      <c r="I16">
+        <v>9.1737582746821103E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>29</v>
       </c>
@@ -4055,8 +4184,14 @@
       <c r="F17">
         <v>6.6516874783178706E-2</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H17">
+        <v>0.14379442561462299</v>
+      </c>
+      <c r="I17">
+        <v>6.06926649217156E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>30</v>
       </c>
@@ -4075,8 +4210,14 @@
       <c r="F18">
         <v>0.20337883120081801</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H18">
+        <v>0.21991637088370999</v>
+      </c>
+      <c r="I18">
+        <v>2.8057730446269601E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>31</v>
       </c>
@@ -4095,8 +4236,14 @@
       <c r="F19">
         <v>0.190294276118984</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H19">
+        <v>0.21734780854119101</v>
+      </c>
+      <c r="I19">
+        <v>1.2678621455846001E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>32</v>
       </c>
@@ -4115,8 +4262,14 @@
       <c r="F20">
         <v>5.2068521068177498E-2</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H20">
+        <v>4.1652001040237099E-2</v>
+      </c>
+      <c r="I20">
+        <v>7.5635218231927107E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>33</v>
       </c>
@@ -4135,8 +4288,14 @@
       <c r="F21">
         <v>0.15547400420750801</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H21">
+        <v>8.5181500851967004E-2</v>
+      </c>
+      <c r="I21">
+        <v>0.13128160966951499</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>34</v>
       </c>
@@ -4155,8 +4314,14 @@
       <c r="F22">
         <v>0.14722870926951601</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H22">
+        <v>2.9762733443890899E-2</v>
+      </c>
+      <c r="I22">
+        <v>0.11521189581253199</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>35</v>
       </c>
@@ -4175,8 +4340,14 @@
       <c r="F23">
         <v>0.13665522794867199</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H23">
+        <v>2.0848362499032099E-2</v>
+      </c>
+      <c r="I23">
+        <v>9.3703241780715402E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>36</v>
       </c>
@@ -4185,7 +4356,7 @@
         <v>0.15054060364663596</v>
       </c>
       <c r="C24" s="1">
-        <f t="shared" ref="C24:H24" si="1">SUM(C14:C23)/10</f>
+        <f t="shared" ref="C24:L24" si="1">SUM(C14:C23)/10</f>
         <v>0.15197388982778576</v>
       </c>
       <c r="D24" s="1">
@@ -4202,9 +4373,25 @@
       </c>
       <c r="G24" s="1">
         <f t="shared" si="1"/>
+        <v>2.8115950309015904E-2</v>
+      </c>
+      <c r="H24" s="1">
+        <f t="shared" si="1"/>
+        <v>0.10609505244754021</v>
+      </c>
+      <c r="I24" s="1">
+        <f t="shared" si="1"/>
+        <v>7.5427684734884676E-2</v>
+      </c>
+      <c r="J24" s="1">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H24" s="1">
+      <c r="K24" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L24" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>

</xml_diff>